<commit_message>
2022.11.16 New way to execute from a parameters file
</commit_message>
<xml_diff>
--- a/Parametros.xlsx
+++ b/Parametros.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25726"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Z_Proyectos\descargas_DIAN\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFBCB789-ED8F-45D9-9146-841CD005C164}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2102C40-B19A-4BAC-AE6C-81A9D633A207}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
+    <sheet name="PARAMETROS" sheetId="1" r:id="rId1"/>
+    <sheet name="LISTAS" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,18 +37,78 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="24">
   <si>
     <t>URL DIAN</t>
   </si>
   <si>
-    <t>FECHA INICIO</t>
-  </si>
-  <si>
-    <t>FECHA FIN</t>
-  </si>
-  <si>
-    <t>https://catalogo-vpfe.dian.gov.co/User/AuthToken?pk=10910094%7C8354408&amp;rk=8354408&amp;token=f428667d-df6b-4267-a260-b2e20d4f8d1c</t>
+    <t>https://catalogo-vpfe.dian.gov.co/User/AuthToken?pk=10910094%7C8354408&amp;rk=8354408&amp;token=936d3eed-1e6b-4a34-9a7d-8a79623485f7</t>
+  </si>
+  <si>
+    <t>Ruta listado excel</t>
+  </si>
+  <si>
+    <t>Fecha inicio</t>
+  </si>
+  <si>
+    <t>Fecha fin</t>
+  </si>
+  <si>
+    <t>Parámetro</t>
+  </si>
+  <si>
+    <t>Valor</t>
+  </si>
+  <si>
+    <t>Observación</t>
+  </si>
+  <si>
+    <t>Ruta donde se encuentran o se encontrarán los archivos .ZIP descargados.</t>
+  </si>
+  <si>
+    <t>Y:\02. CONTABILIDAD\1 CONTADOR\2 CLAUDIA  PATRICIA GOMEZ SALAZAR\CLAUDIA FACT ELECTRONICAS 2022\RADIAN\10. 31 OCT AL 11 NOV 2022</t>
+  </si>
+  <si>
+    <t>Y:\02. CONTABILIDAD\1 CONTADOR\2 CLAUDIA  PATRICIA GOMEZ SALAZAR\CLAUDIA FACT ELECTRONICAS 2022\RADIAN\10. 31 OCT AL 11 NOV 2022\Documentos.xlsx</t>
+  </si>
+  <si>
+    <t>Tipo de ejecución</t>
+  </si>
+  <si>
+    <t>Opciones</t>
+  </si>
+  <si>
+    <t>SI</t>
+  </si>
+  <si>
+    <t>NO</t>
+  </si>
+  <si>
+    <t>Descarga + Clasificación</t>
+  </si>
+  <si>
+    <t>Descarga</t>
+  </si>
+  <si>
+    <t>Clasificación</t>
+  </si>
+  <si>
+    <t>Descarga desde excel</t>
+  </si>
+  <si>
+    <t>Si la descarga de facturas se hará desde un listado de excel o interactuando con la página de la DIAN.</t>
+  </si>
+  <si>
+    <t>Debe ser la ruta exacta al archivo, debe terminar en .xlsx</t>
+  </si>
+  <si>
+    <t>Si la descarga se hará interactuando con la página de la DIAN.</t>
+  </si>
+  <si>
+    <t>Descarga de facturas y/o clasificación según forma de pago (Contado-Crédito)</t>
+  </si>
+  <si>
+    <t>Ruta ZIPs</t>
   </si>
 </sst>
 </file>
@@ -79,12 +140,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -100,11 +167,22 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -386,47 +464,176 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="125.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.28515625" style="6" customWidth="1"/>
+    <col min="3" max="3" width="89.85546875" customWidth="1"/>
+    <col min="4" max="4" width="125.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" s="4">
+        <f ca="1">+B7-30</f>
+        <v>44850</v>
+      </c>
+      <c r="C6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7" s="4">
+        <f ca="1">+TODAY()-1</f>
+        <v>44880</v>
+      </c>
+      <c r="C7" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B8" s="5" t="s">
         <v>1</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="2">
-        <f ca="1">+B2-30</f>
-        <v>44830</v>
-      </c>
-      <c r="B2" s="2">
-        <f ca="1">+TODAY()-1</f>
-        <v>44860</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>3</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1" xr:uid="{98E27248-B32D-4352-8220-4C7E92F60D56}"/>
+    <hyperlink ref="B8" r:id="rId1" xr:uid="{CD30BBAB-D18C-4375-ABAA-1F420C85DF6C}"/>
   </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{A7FD9B05-8E7E-4ACB-B79B-7EBF5FD5DD10}">
+          <x14:formula1>
+            <xm:f>LISTAS!$A$2:$A$4</xm:f>
+          </x14:formula1>
+          <xm:sqref>B2</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{C5A93500-F615-4FF2-BC12-ADEFD55EDA9C}">
+          <x14:formula1>
+            <xm:f>LISTAS!$B$2:$B$3</xm:f>
+          </x14:formula1>
+          <xm:sqref>B3</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6422D0D3-FE55-49B8-A15F-655B8CC8A4E0}">
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="21.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>